<commit_message>
add score to ply func result
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\88691\Desktop\交大專題\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23315777-D545-4C54-B112-2FA93178FDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1566B2-0FDC-4F7C-8997-A600279381BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="abcut3.18" sheetId="1" r:id="rId1"/>
     <sheet name="startimax 3.19" sheetId="2" r:id="rId2"/>
+    <sheet name="add scoreply func 3.20" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>1024(%)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,6 +102,10 @@
   </si>
   <si>
     <t xml:space="preserve">worst_rate:0.7 total:10 (add score to ply func) 30000:0 1000000:1 else 2 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time(sec)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -643,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{383892EE-57D4-48B5-9900-02FD93548A48}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H12"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -655,7 +660,7 @@
     <col min="4" max="5" width="35" customWidth="1"/>
     <col min="6" max="6" width="30.625" customWidth="1"/>
     <col min="7" max="7" width="29.875" customWidth="1"/>
-    <col min="8" max="8" width="47.625" customWidth="1"/>
+    <col min="8" max="8" width="65.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -677,9 +682,6 @@
       <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -700,9 +702,7 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -723,9 +723,7 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -746,9 +744,7 @@
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -769,9 +765,7 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -792,9 +786,7 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -815,9 +807,7 @@
       <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -838,9 +828,7 @@
       <c r="F8" s="1">
         <v>0.8</v>
       </c>
-      <c r="H8" s="1">
-        <v>0.8</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -855,9 +843,7 @@
       <c r="F9" s="1">
         <v>0.2</v>
       </c>
-      <c r="H9" s="1">
-        <v>0.2</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -872,9 +858,7 @@
       <c r="F10" s="2">
         <v>152519</v>
       </c>
-      <c r="H10" s="2">
-        <v>152519</v>
-      </c>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -889,25 +873,19 @@
       <c r="F11">
         <v>225964</v>
       </c>
-      <c r="H11">
-        <v>225964</v>
-      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D12">
-        <v>399792</v>
+        <v>399.79199999999997</v>
       </c>
       <c r="E12">
-        <v>6841</v>
+        <v>6.8410000000000002</v>
       </c>
       <c r="F12">
-        <v>240015</v>
-      </c>
-      <c r="H12">
-        <v>240015</v>
+        <v>240.01499999999999</v>
       </c>
     </row>
   </sheetData>
@@ -915,4 +893,117 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D02903-6163-430F-8949-9C71061F9B7D}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView zoomScale="108" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.375" customWidth="1"/>
+    <col min="2" max="2" width="62.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <v>123664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>178872</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>2974.1860000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>